<commit_message>
add local storage and DOM manipulation to CIT proj
</commit_message>
<xml_diff>
--- a/CIT261/Other Assignments/CIT261-G1-Topics.xlsx
+++ b/CIT261/Other Assignments/CIT261-G1-Topics.xlsx
@@ -1,22 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryandockstader/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ry\Documents\Learning\BYUI\GITHUB\CIT261\Other Assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84633A4F-7BFA-8548-BD27-26CC8302A408}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB1366E-F63F-4A4F-935D-56C0D9FE820A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -162,7 +170,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -194,8 +202,22 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -214,6 +236,16 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -224,10 +256,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -236,13 +270,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="2" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -562,16 +600,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.5" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.83203125" customWidth="1"/>
-    <col min="6" max="6" width="16.5" customWidth="1"/>
+    <col min="1" max="1" width="39.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -591,7 +629,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -607,7 +645,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -619,7 +657,7 @@
       </c>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -632,7 +670,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -644,7 +682,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -658,7 +696,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -670,7 +708,7 @@
       </c>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -682,7 +720,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
@@ -694,7 +732,7 @@
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
@@ -708,7 +746,7 @@
       </c>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
@@ -722,7 +760,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
@@ -736,7 +774,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>25</v>
       </c>
@@ -748,7 +786,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>27</v>
       </c>
@@ -760,7 +798,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="B15" s="5">
         <f t="shared" ref="B15:F15" si="0">COUNTA(B2:B14)</f>
@@ -793,90 +831,90 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="108.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="108.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="47" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:3" ht="46.5" x14ac:dyDescent="0.7">
+      <c r="A1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-    </row>
-    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>37</v>
       </c>
@@ -887,18 +925,18 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>39</v>
       </c>
@@ -909,7 +947,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>40</v>
       </c>
@@ -920,7 +958,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>41</v>
       </c>
@@ -931,7 +969,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>42</v>
       </c>
@@ -942,7 +980,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>43</v>
       </c>
@@ -953,7 +991,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
add more CSS transitions
</commit_message>
<xml_diff>
--- a/CIT261/Other Assignments/CIT261-G1-Topics.xlsx
+++ b/CIT261/Other Assignments/CIT261-G1-Topics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ry\Documents\Learning\BYUI\GITHUB\CIT261\Other Assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB1366E-F63F-4A4F-935D-56C0D9FE820A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4906C4-58D9-48D7-9B59-EB68468CD875}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-2280" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="45">
   <si>
     <t>Topic</t>
   </si>
@@ -170,7 +170,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -209,15 +209,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -241,11 +234,6 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -256,31 +244,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -639,8 +623,8 @@
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
@@ -649,13 +633,13 @@
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
       <c r="D3" s="2"/>
       <c r="E3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="4"/>
+      <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -668,45 +652,45 @@
         <v>8</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="4"/>
+      <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="3"/>
       <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="3"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="4"/>
+      <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="3"/>
       <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="4"/>
+      <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
@@ -716,35 +700,35 @@
       <c r="C8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="4"/>
+      <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="4"/>
+      <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="4"/>
+      <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -753,8 +737,8 @@
       <c r="B11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
         <v>15</v>
@@ -764,8 +748,8 @@
       <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
       <c r="D12" s="2"/>
       <c r="E12" s="3" t="s">
         <v>7</v>
@@ -781,42 +765,42 @@
       <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="4"/>
+      <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4">
         <f t="shared" ref="B15:F15" si="0">COUNTA(B2:B14)</f>
         <v>4</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -831,7 +815,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -849,101 +833,101 @@
       <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="6" t="s">
         <v>7</v>
       </c>
     </row>
@@ -991,14 +975,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="6" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>